<commit_message>
feat: math 1-3 to one file
</commit_message>
<xml_diff>
--- a/Математика/ДЗ_1.xlsx
+++ b/Математика/ДЗ_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony_\OneDrive\Документы\omstu-works-2\Математика\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BA83B0-4340-49B2-9611-A91C2D0A0708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A970587-56B2-4F9C-8EBF-9DFA8D1CAF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{1CF31AF0-7197-4C31-9E7C-A0D24E014F79}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="1" xr2:uid="{1CF31AF0-7197-4C31-9E7C-A0D24E014F79}"/>
   </bookViews>
   <sheets>
     <sheet name="метод половинного деления" sheetId="1" r:id="rId1"/>
@@ -4849,7 +4849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A39C61-D37F-4390-8BB5-1D2231BEB643}">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
@@ -7892,7 +7892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690C8C8E-D45F-487D-9FBC-F5553011C478}">
   <dimension ref="A1:W103"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
@@ -8975,7 +8975,7 @@
         <v>1.59375</v>
       </c>
       <c r="T30" s="1" t="str">
-        <f t="shared" ref="T30:T35" si="7">IF(ABS(N30)&lt;(2*$W$29), "ВСЁ","ЕЩЁ")</f>
+        <f t="shared" ref="T30:T33" si="7">IF(ABS(N30)&lt;(2*$W$29), "ВСЁ","ЕЩЁ")</f>
         <v>ЕЩЁ</v>
       </c>
     </row>
@@ -9015,35 +9015,35 @@
         <v>2</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" ref="L31:L35" si="8">L30+Q30</f>
+        <f t="shared" ref="L31:L33" si="8">L30+Q30</f>
         <v>1.5057681114028041</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" ref="M31:M35" si="9">M30+R30</f>
+        <f t="shared" ref="M31:M33" si="9">M30+R30</f>
         <v>1.5517947816718816</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" ref="N31:N35" si="10">M31-L31</f>
+        <f t="shared" ref="N31:N33" si="10">M31-L31</f>
         <v>4.6026670269077474E-2</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" ref="O31:O35" si="11">LN(L31)-1/(L31^2)</f>
+        <f t="shared" ref="O31:O33" si="11">LN(L31)-1/(L31^2)</f>
         <v>-3.1742778931296567E-2</v>
       </c>
       <c r="P31" s="1">
-        <f t="shared" ref="P31:P35" si="12">LN(M31)-1/(M31^2)</f>
+        <f t="shared" ref="P31:P33" si="12">LN(M31)-1/(M31^2)</f>
         <v>2.4141354810916116E-2</v>
       </c>
       <c r="Q31" s="1">
-        <f t="shared" ref="Q31:Q35" si="13">-O31/S31</f>
+        <f t="shared" ref="Q31:Q33" si="13">-O31/S31</f>
         <v>2.5395819304983473E-2</v>
       </c>
       <c r="R31" s="1">
-        <f t="shared" ref="R31:R35" si="14">-(P31*N31)/(P31-O31)</f>
+        <f t="shared" ref="R31:R33" si="14">-(P31*N31)/(P31-O31)</f>
         <v>-1.9883034831611374E-2</v>
       </c>
       <c r="S31" s="1">
-        <f t="shared" ref="S31:S35" si="15">1/L31+2/(L31^3)</f>
+        <f t="shared" ref="S31:S33" si="15">1/L31+2/(L31^3)</f>
         <v>1.2499214358903403</v>
       </c>
       <c r="T31" s="1" t="str">

</xml_diff>